<commit_message>
Einheiten und Combobox Längenbeschrenkung
</commit_message>
<xml_diff>
--- a/TorqueMonitoring/files/SchnittdatenControl.xlsx
+++ b/TorqueMonitoring/files/SchnittdatenControl.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\torge\source\repos\TorqueMonitoring\TorqueMonitoring\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jan\Source\Repos\torquemonitoring\TorqueMonitoring\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE58917-8E18-42D0-B0B8-3F2D39853699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6ED6C87-FCA6-493C-B88F-804A2E5B7D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29985" yWindow="1350" windowWidth="21600" windowHeight="12645" xr2:uid="{2503F9C7-F3A8-A644-B2DD-9F337C9EE520}"/>
+    <workbookView xWindow="-27750" yWindow="4020" windowWidth="27090" windowHeight="13815" xr2:uid="{2503F9C7-F3A8-A644-B2DD-9F337C9EE520}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,15 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1546,25 +1537,25 @@
       <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.8984375" defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="2" width="10.625" customWidth="1"/>
-    <col min="3" max="3" width="38.25" customWidth="1"/>
-    <col min="4" max="4" width="27.375" customWidth="1"/>
-    <col min="5" max="5" width="68.75" customWidth="1"/>
-    <col min="6" max="6" width="12.375" customWidth="1"/>
+    <col min="2" max="2" width="10.59765625" customWidth="1"/>
+    <col min="3" max="3" width="38.19921875" customWidth="1"/>
+    <col min="4" max="4" width="27.3984375" customWidth="1"/>
+    <col min="5" max="5" width="68.69921875" customWidth="1"/>
+    <col min="6" max="6" width="12.3984375" customWidth="1"/>
     <col min="7" max="7" width="10.5" customWidth="1"/>
-    <col min="8" max="8" width="18.625" customWidth="1"/>
-    <col min="9" max="9" width="20.875" customWidth="1"/>
+    <col min="8" max="8" width="18.59765625" customWidth="1"/>
+    <col min="9" max="9" width="20.8984375" customWidth="1"/>
     <col min="10" max="10" width="12.5" customWidth="1"/>
     <col min="11" max="11" width="10.5" customWidth="1"/>
-    <col min="12" max="12" width="17.125" customWidth="1"/>
+    <col min="12" max="12" width="17.09765625" customWidth="1"/>
     <col min="13" max="13" width="20.5" customWidth="1"/>
-    <col min="14" max="14" width="12.125" customWidth="1"/>
+    <col min="14" max="14" width="12.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:13" ht="16.5" thickBot="1"/>
-    <row r="6" spans="2:13" ht="17.25" thickTop="1" thickBot="1">
+    <row r="5" spans="2:13" ht="16.2" thickBot="1"/>
+    <row r="6" spans="2:13" ht="16.8" thickTop="1" thickBot="1">
       <c r="B6" s="13" t="s">
         <v>0</v>
       </c>
@@ -1572,18 +1563,18 @@
         <v>1</v>
       </c>
       <c r="D6" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" ht="17.25" thickTop="1" thickBot="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" ht="16.8" thickTop="1" thickBot="1">
       <c r="B7" s="15"/>
       <c r="C7" s="16" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="2:13" ht="17.25" thickTop="1" thickBot="1"/>
-    <row r="9" spans="2:13" ht="17.25" thickTop="1" thickBot="1">
+    <row r="8" spans="2:13" ht="16.8" thickTop="1" thickBot="1"/>
+    <row r="9" spans="2:13" ht="16.8" thickTop="1" thickBot="1">
       <c r="B9" s="13" t="s">
         <v>21</v>
       </c>
@@ -1595,7 +1586,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="10" spans="2:13" ht="17.25" thickTop="1" thickBot="1">
+    <row r="10" spans="2:13" ht="16.8" thickTop="1" thickBot="1">
       <c r="B10" s="17"/>
       <c r="C10" s="18" t="s">
         <v>26</v>
@@ -1605,7 +1596,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="2:13" ht="16.5" thickBot="1">
+    <row r="11" spans="2:13" ht="16.2" thickBot="1">
       <c r="B11" s="17"/>
       <c r="C11" s="18" t="s">
         <v>30</v>
@@ -1615,7 +1606,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="12" spans="2:13" ht="16.5" thickBot="1">
+    <row r="12" spans="2:13" ht="16.2" thickBot="1">
       <c r="B12" s="17"/>
       <c r="C12" s="18" t="s">
         <v>34</v>
@@ -1625,7 +1616,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="2:13" ht="16.5" thickBot="1">
+    <row r="13" spans="2:13" ht="16.2" thickBot="1">
       <c r="B13" s="15"/>
       <c r="C13" s="16" t="s">
         <v>38</v>
@@ -1635,8 +1626,8 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="14" spans="2:13" ht="16.5" thickTop="1"/>
-    <row r="15" spans="2:13" ht="16.5" thickBot="1">
+    <row r="14" spans="2:13" ht="16.2" thickTop="1"/>
+    <row r="15" spans="2:13" ht="16.2" thickBot="1">
       <c r="L15" t="s">
         <v>42</v>
       </c>
@@ -1644,7 +1635,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="2:13" ht="16.5" thickTop="1">
+    <row r="16" spans="2:13" ht="16.2" thickTop="1">
       <c r="B16" s="137" t="s">
         <v>2</v>
       </c>
@@ -1693,7 +1684,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="16.5" thickBot="1">
+    <row r="18" spans="2:10" ht="16.2" thickBot="1">
       <c r="B18" s="139"/>
       <c r="C18" s="151"/>
       <c r="D18" s="148"/>
@@ -1708,7 +1699,7 @@
       <c r="I18" s="148"/>
       <c r="J18" s="145"/>
     </row>
-    <row r="19" spans="2:10" ht="16.5" thickTop="1">
+    <row r="19" spans="2:10" ht="16.2" thickTop="1">
       <c r="B19" s="110">
         <v>1</v>
       </c>
@@ -1729,7 +1720,7 @@
       </c>
       <c r="H19" s="23">
         <f>(0.025*$D$6)/2</f>
-        <v>0.125</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="I19" s="23">
         <v>1500</v>
@@ -1753,7 +1744,7 @@
       </c>
       <c r="H20" s="27">
         <f>(0.025*$D$6)/2</f>
-        <v>0.125</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="I20" s="27">
         <v>1700</v>
@@ -1777,7 +1768,7 @@
       </c>
       <c r="H21" s="27">
         <f t="shared" ref="H21:H27" si="0">(0.01*$D$6)/2</f>
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="I21" s="27">
         <v>2000</v>
@@ -1801,7 +1792,7 @@
       </c>
       <c r="H22" s="27">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="I22" s="27">
         <v>2200</v>
@@ -1825,7 +1816,7 @@
       </c>
       <c r="H23" s="27">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="I23" s="27">
         <v>2500</v>
@@ -1834,7 +1825,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="16.5" thickBot="1">
+    <row r="24" spans="2:10" ht="16.2" thickBot="1">
       <c r="B24" s="112"/>
       <c r="C24" s="115"/>
       <c r="D24" s="103"/>
@@ -1849,7 +1840,7 @@
       </c>
       <c r="H24" s="51">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="I24" s="51">
         <v>3000</v>
@@ -1858,7 +1849,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="16.5" thickTop="1">
+    <row r="25" spans="2:10" ht="16.2" thickTop="1">
       <c r="B25" s="134">
         <v>2</v>
       </c>
@@ -1879,7 +1870,7 @@
       </c>
       <c r="H25" s="59">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="I25" s="59">
         <v>1800</v>
@@ -1903,7 +1894,7 @@
       </c>
       <c r="H26" s="31">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="I26" s="31">
         <v>2000</v>
@@ -1912,7 +1903,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="27" spans="2:10" ht="16.5" thickBot="1">
+    <row r="27" spans="2:10" ht="16.2" thickBot="1">
       <c r="B27" s="136"/>
       <c r="C27" s="133"/>
       <c r="D27" s="130"/>
@@ -1927,7 +1918,7 @@
       </c>
       <c r="H27" s="63">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="I27" s="63">
         <v>2400</v>
@@ -1936,7 +1927,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="28" spans="2:10" ht="16.5" thickTop="1">
+    <row r="28" spans="2:10" ht="16.2" thickTop="1">
       <c r="B28" s="116">
         <v>3</v>
       </c>
@@ -1957,7 +1948,7 @@
       </c>
       <c r="H28" s="55">
         <f>(0.025*$D$6)/2</f>
-        <v>0.125</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="I28" s="55">
         <v>800</v>
@@ -1981,7 +1972,7 @@
       </c>
       <c r="H29" s="9">
         <f>(0.025*$D$6)/2</f>
-        <v>0.125</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="I29" s="9">
         <v>950</v>
@@ -2005,7 +1996,7 @@
       </c>
       <c r="H30" s="9">
         <f>(0.025*$D$6)/2</f>
-        <v>0.125</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="I30" s="9">
         <v>1200</v>
@@ -2014,7 +2005,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="31" spans="2:10" ht="16.5" thickBot="1">
+    <row r="31" spans="2:10" ht="16.2" thickBot="1">
       <c r="B31" s="118"/>
       <c r="C31" s="121"/>
       <c r="D31" s="106"/>
@@ -2029,7 +2020,7 @@
       </c>
       <c r="H31" s="67">
         <f>(0.02*$D$6)/2</f>
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="I31" s="67">
         <v>1400</v>
@@ -2038,7 +2029,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="32" spans="2:10" ht="16.5" thickTop="1">
+    <row r="32" spans="2:10" ht="16.2" thickTop="1">
       <c r="B32" s="122">
         <v>4</v>
       </c>
@@ -2059,7 +2050,7 @@
       </c>
       <c r="H32" s="75">
         <f>(0.025*$D$6)/2</f>
-        <v>0.125</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="I32" s="75">
         <v>350</v>
@@ -2083,7 +2074,7 @@
       </c>
       <c r="H33" s="35">
         <f>(0.025*$D$6)/2</f>
-        <v>0.125</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="I33" s="35">
         <v>600</v>
@@ -2107,7 +2098,7 @@
       </c>
       <c r="H34" s="35">
         <f>(0.015*$D$6)/2</f>
-        <v>7.4999999999999997E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="I34" s="35">
         <v>600</v>
@@ -2131,7 +2122,7 @@
       </c>
       <c r="H35" s="35">
         <f>(0.015*$D$6)/2</f>
-        <v>7.4999999999999997E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="I35" s="35">
         <v>700</v>
@@ -2155,7 +2146,7 @@
       </c>
       <c r="H36" s="35">
         <f>(0.045*$D$6)/2</f>
-        <v>0.22499999999999998</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="I36" s="35">
         <v>550</v>
@@ -2164,7 +2155,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="37" spans="2:10" ht="16.5" thickBot="1">
+    <row r="37" spans="2:10" ht="16.2" thickBot="1">
       <c r="B37" s="124"/>
       <c r="C37" s="127"/>
       <c r="D37" s="109"/>
@@ -2179,7 +2170,7 @@
       </c>
       <c r="H37" s="79">
         <f>(0.025*$D$6)/2</f>
-        <v>0.125</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="I37" s="79">
         <v>1000</v>
@@ -2188,7 +2179,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="38" spans="2:10" ht="16.5" thickTop="1">
+    <row r="38" spans="2:10" ht="16.2" thickTop="1">
       <c r="B38" s="161">
         <v>5</v>
       </c>
@@ -2320,7 +2311,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="44" spans="2:10" ht="16.5" thickBot="1">
+    <row r="44" spans="2:10" ht="16.2" thickBot="1">
       <c r="B44" s="163"/>
       <c r="C44" s="166"/>
       <c r="D44" s="169"/>
@@ -2341,7 +2332,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="45" spans="2:10" ht="16.5" thickTop="1">
+    <row r="45" spans="2:10" ht="16.2" thickTop="1">
       <c r="B45" s="170">
         <v>6</v>
       </c>
@@ -2410,7 +2401,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="48" spans="2:10" ht="16.5" thickBot="1">
+    <row r="48" spans="2:10" ht="16.2" thickBot="1">
       <c r="B48" s="172"/>
       <c r="C48" s="175"/>
       <c r="D48" s="178"/>
@@ -2431,7 +2422,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="49" spans="2:10" ht="16.5" thickTop="1">
+    <row r="49" spans="2:10" ht="16.2" thickTop="1">
       <c r="B49" s="152">
         <v>7</v>
       </c>
@@ -2452,7 +2443,7 @@
       </c>
       <c r="H49" s="87">
         <f>(0.025*$D$6)/2</f>
-        <v>0.125</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="I49" s="87">
         <v>150</v>
@@ -2482,7 +2473,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="51" spans="2:10" ht="16.5" thickBot="1">
+    <row r="51" spans="2:10" ht="16.2" thickBot="1">
       <c r="B51" s="154"/>
       <c r="C51" s="157"/>
       <c r="D51" s="160"/>
@@ -2503,7 +2494,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="52" spans="2:10" ht="16.5" thickTop="1">
+    <row r="52" spans="2:10" ht="16.2" thickTop="1">
       <c r="D52" t="s">
         <v>73</v>
       </c>

</xml_diff>